<commit_message>
ajuste de los números telefónicos del excel
</commit_message>
<xml_diff>
--- a/data/fake_list.xlsx
+++ b/data/fake_list.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mcorr\OneDrive\Documentos\ESTUDIO_PROGRAMACIÓN\Proyecto_1\villa_fc\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\proyectospersonales\villa_fc\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F32DF6D4-C9E2-4F1B-BAD3-66EBEC68EF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{562B6D73-AAD2-464B-B2DF-3D7D12030574}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="735" yWindow="735" windowWidth="15375" windowHeight="7875" xr2:uid="{87A0AE98-CB7C-4DF0-BC68-4A0B04C49605}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{87A0AE98-CB7C-4DF0-BC68-4A0B04C49605}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
   <si>
     <t>NOMBRE</t>
   </si>
@@ -39,88 +39,70 @@
     <t>ULTIMO_PAGO</t>
   </si>
   <si>
-    <t xml:space="preserve">Hugo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Martín </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lucas </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mateo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leo </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniel </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Alejandro </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pablo </t>
-  </si>
-  <si>
-    <t>Manuel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Álvaro </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adrián </t>
-  </si>
-  <si>
-    <t xml:space="preserve">David </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mario </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Enzo </t>
-  </si>
-  <si>
-    <t>Rodriguez</t>
-  </si>
-  <si>
-    <t>Martinez</t>
-  </si>
-  <si>
-    <t>Garcia</t>
-  </si>
-  <si>
-    <t>Gomez</t>
-  </si>
-  <si>
-    <t>Lopez</t>
-  </si>
-  <si>
-    <t>Gonzalez</t>
-  </si>
-  <si>
-    <t>Hernandez</t>
-  </si>
-  <si>
-    <t>Sanchez</t>
-  </si>
-  <si>
-    <t>Perez</t>
-  </si>
-  <si>
-    <t>Valencia</t>
-  </si>
-  <si>
-    <t>Duque</t>
-  </si>
-  <si>
-    <t>Perdomo</t>
-  </si>
-  <si>
-    <t>Cardona</t>
-  </si>
-  <si>
-    <t>Arango</t>
+    <t>Daniela</t>
+  </si>
+  <si>
+    <t>Villamizar</t>
+  </si>
+  <si>
+    <t>Botero</t>
+  </si>
+  <si>
+    <t>Juan</t>
+  </si>
+  <si>
+    <t>Cristian</t>
+  </si>
+  <si>
+    <t>Solarte</t>
+  </si>
+  <si>
+    <t>Julian</t>
+  </si>
+  <si>
+    <t>Aristizabal</t>
+  </si>
+  <si>
+    <t>Londoño</t>
+  </si>
+  <si>
+    <t>Mauricio</t>
+  </si>
+  <si>
+    <t>Herrera</t>
+  </si>
+  <si>
+    <t>Esteban</t>
+  </si>
+  <si>
+    <t>Meneses</t>
+  </si>
+  <si>
+    <t>Carlos</t>
+  </si>
+  <si>
+    <t>Paraco</t>
+  </si>
+  <si>
+    <t>Alejandra</t>
+  </si>
+  <si>
+    <t>Ruiz</t>
+  </si>
+  <si>
+    <t>Bustos</t>
+  </si>
+  <si>
+    <t>Laura</t>
+  </si>
+  <si>
+    <t>Hoyos</t>
+  </si>
+  <si>
+    <t>Manuela</t>
+  </si>
+  <si>
+    <t>Rojas</t>
   </si>
 </sst>
 </file>
@@ -483,10 +465,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37839F57-F0AB-432C-9ADF-25E7EDB61B14}">
-  <dimension ref="A1:E15"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -516,10 +498,10 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>3015698423</v>
+        <v>3218490916</v>
       </c>
       <c r="D2" s="1">
         <v>44604</v>
@@ -527,185 +509,157 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="C3">
-        <v>3215698521</v>
+        <v>3218748814</v>
       </c>
       <c r="D3" s="1">
-        <v>44636</v>
+        <v>44605</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>3136482105</v>
+        <v>3148227994</v>
       </c>
       <c r="D4" s="1">
-        <v>45592</v>
+        <v>44606</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="C5">
-        <v>3145678015</v>
+        <v>3046145922</v>
       </c>
       <c r="D5" s="1">
-        <v>45550</v>
+        <v>44607</v>
       </c>
       <c r="E5" s="3"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="C6">
-        <v>3116254231</v>
+        <v>3163610054</v>
       </c>
       <c r="D6" s="1">
-        <v>45147</v>
+        <v>44608</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="C7">
-        <v>3002016952</v>
+        <v>3117754781</v>
       </c>
       <c r="D7" s="1">
-        <v>45099</v>
+        <v>44609</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C8">
-        <v>3023519754</v>
+        <v>3108017554</v>
       </c>
       <c r="D8" s="1">
-        <v>45614</v>
+        <v>44610</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B9" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C9">
-        <v>3015698567</v>
+        <v>3188288098</v>
       </c>
       <c r="D9" s="1">
-        <v>45405</v>
+        <v>44611</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C10">
-        <v>3236521693</v>
+        <v>3167357054</v>
       </c>
       <c r="D10" s="1">
-        <v>44660</v>
+        <v>44612</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="C11">
-        <v>3189657436</v>
+        <v>3164224295</v>
       </c>
       <c r="D11" s="1">
-        <v>45091</v>
+        <v>44613</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="C12">
-        <v>3185201260</v>
+        <v>3113829197</v>
       </c>
       <c r="D12" s="1">
-        <v>45498</v>
+        <v>44614</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C13">
-        <v>3224697851</v>
+        <v>3114244572</v>
       </c>
       <c r="D13" s="1">
-        <v>45346</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C14">
-        <v>3230569853</v>
-      </c>
-      <c r="D14" s="1">
-        <v>45227</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15">
-        <v>3045876320</v>
-      </c>
-      <c r="D15" s="1">
-        <v>45181</v>
+        <v>44615</v>
       </c>
     </row>
   </sheetData>

</xml_diff>